<commit_message>
trying to added table to xlsx
</commit_message>
<xml_diff>
--- a/docs/cryptotidbits.xlsx
+++ b/docs/cryptotidbits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/17682d9813a3865f/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swima\projects\portfolio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{283B36C6-82C6-4AD2-8114-6DC3BC725E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EED4681C-2AEC-4BDB-B775-3952CC7EA861}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D63B31-3417-4FD0-B943-DE752CF844FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8085" yWindow="690" windowWidth="22155" windowHeight="13215" xr2:uid="{288A868F-4980-44F9-AD20-5928230AFE10}"/>
+    <workbookView xWindow="32175" yWindow="975" windowWidth="21600" windowHeight="11385" xr2:uid="{288A868F-4980-44F9-AD20-5928230AFE10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1014,7 +1014,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1027,8 +1034,16 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B67931A4-9B7E-4267-AB5D-C89224F6C230}" name="Table1" displayName="Table1" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101" xr:uid="{B67931A4-9B7E-4267-AB5D-C89224F6C230}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8884A4FD-E0C6-4CE3-B9D8-25C78D89603C}" name="Title"/>
+    <tableColumn id="2" xr3:uid="{AB487AAB-708C-4322-A211-0A87DB9200C5}" name="Word" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1D6F051D-1004-4964-A875-38ADDB0EDA0A}" name="Tidbit" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1330,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D9B3CF-CD8F-47A4-AD80-1BC9E86E89DE}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B41" sqref="B33:B41"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,5 +2470,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>